<commit_message>
First working version of StackBuilder Addin with per row computations...
</commit_message>
<xml_diff>
--- a/Sources/CustomProjects/treeDiM.StackBuilder.ExcelAddIn/Data/Catalogtikamoon.xlsx
+++ b/Sources/CustomProjects/treeDiM.StackBuilder.ExcelAddIn/Data/Catalogtikamoon.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy\Desktop\doc mat tika\Catalogue stackbuilder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\StackBuilder\Sources\CustomProjects\treeDiM.StackBuilder.ExcelAddIn\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF210E6-7588-4067-9DB0-2D49999BB474}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="14355" windowHeight="4680"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="14355" windowHeight="4680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="1" r:id="rId1"/>
@@ -4943,7 +4944,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -5070,7 +5071,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5145,6 +5146,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5180,6 +5198,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5355,14 +5390,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L802"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="82.28515625" bestFit="1" customWidth="1"/>
@@ -21922,7 +21957,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L802">
+  <autoFilter ref="A1:L802" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A2:L802">
       <sortCondition ref="A1:A802"/>
     </sortState>
@@ -21933,14 +21968,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
@@ -21984,7 +22019,7 @@
         <v>800</v>
       </c>
       <c r="E2" s="5">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="F2" s="6">
         <v>20</v>
@@ -22005,7 +22040,7 @@
         <v>1140</v>
       </c>
       <c r="E3" s="5">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="F3" s="6">
         <v>20</v>
@@ -22864,14 +22899,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J802"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
@@ -23263,14 +23298,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
@@ -24213,14 +24248,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.85546875" bestFit="1" customWidth="1"/>
@@ -25152,14 +25187,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -25215,14 +25250,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" customWidth="1"/>
@@ -26373,14 +26408,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
@@ -27218,14 +27253,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>

</xml_diff>